<commit_message>
added a small example with damages from emissions
in misc/damagesFromEmissions.ipynb
</commit_message>
<xml_diff>
--- a/Misc/Data/mBasicInt1.xlsx
+++ b/Misc/Data/mBasicInt1.xlsx
@@ -547,7 +547,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -770,7 +770,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>